<commit_message>
updated covid GDP impacts
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/GDPGR/GDP Growth Rates.xlsx
+++ b/InputData/ctrl-settings/GDPGR/GDP Growth Rates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iamho\Dropbox\Energy Innovation\InputData_Complete\ctrl-settings\GDPGR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\South Korea\eps-southkorea\InputData\ctrl-settings\GDPGR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE7EE48-E7EE-40CA-AED9-B7AC664ACFDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DBA3ED3-992B-450F-B1D9-A78DFA335EE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12740" yWindow="250" windowWidth="12720" windowHeight="13230" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
   <si>
     <t>About</t>
   </si>
@@ -174,6 +174,15 @@
   <si>
     <t>GDP growth rate of 2020 and 2030</t>
     <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Calculated covid recession</t>
+  </si>
+  <si>
+    <t>2020 - covid</t>
+  </si>
+  <si>
+    <t>2020 - bau</t>
   </si>
 </sst>
 </file>
@@ -181,15 +190,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="176" formatCode="0.0%"/>
-    <numFmt numFmtId="177" formatCode="0.000"/>
-    <numFmt numFmtId="178" formatCode="0.0000_);[Red]\(0.0000\)"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0000_);[Red]\(0.0000\)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -197,14 +206,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -212,7 +221,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -220,19 +229,19 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -251,6 +260,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -266,7 +281,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -285,22 +300,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="백분율" xfId="1" builtinId="5"/>
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
-    <cellStyle name="하이퍼링크" xfId="2" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -584,22 +610,22 @@
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="52.58203125" customWidth="1"/>
+    <col min="2" max="2" width="52.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -607,159 +633,159 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2">
       <c r="B5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2">
       <c r="B6" s="14" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2">
       <c r="B7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2">
       <c r="B8" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2">
       <c r="B9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:2">
       <c r="A26" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B26" s="2"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:2">
       <c r="A36" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B36" s="5"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:2">
       <c r="A38" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:2">
       <c r="A39" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:2">
       <c r="A40" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:2">
       <c r="A41" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:2">
       <c r="A42" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:2">
       <c r="A43" t="s">
         <v>15</v>
       </c>
@@ -775,20 +801,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="15.58203125" customWidth="1"/>
-    <col min="2" max="2" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="15.58203125" customWidth="1"/>
-    <col min="7" max="7" width="8.75" customWidth="1"/>
+    <col min="1" max="1" width="15.54296875" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="15.54296875" customWidth="1"/>
+    <col min="7" max="7" width="8.7265625" customWidth="1"/>
+    <col min="8" max="8" width="14.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10">
       <c r="B1" s="18" t="s">
         <v>38</v>
       </c>
@@ -803,7 +830,7 @@
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" ht="29">
       <c r="B2" t="s">
         <v>36</v>
       </c>
@@ -818,69 +845,87 @@
       </c>
       <c r="F2" s="13"/>
       <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A3">
+      <c r="H2" s="21"/>
+      <c r="I2" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="29">
+      <c r="A3" s="19">
         <v>2020</v>
       </c>
-      <c r="B3" s="16">
-        <v>8.0000000000000071E-3</v>
-      </c>
-      <c r="C3">
-        <v>1.0000000000000002E-3</v>
-      </c>
-      <c r="D3" s="16">
-        <v>3.3000000000000002E-2</v>
-      </c>
-      <c r="E3">
+      <c r="B3" s="20">
+        <v>4.4900000000000001E-3</v>
+      </c>
+      <c r="C3" s="19">
+        <v>-8.9999999999999993E-3</v>
+      </c>
+      <c r="D3" s="20">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="E3" s="19">
         <v>0.02</v>
       </c>
       <c r="F3" s="13"/>
       <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A4">
+      <c r="H3" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" s="23">
+        <f>C3</f>
+        <v>-8.9999999999999993E-3</v>
+      </c>
+      <c r="J3" s="23">
+        <f>E3</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="19">
         <v>2021</v>
       </c>
-      <c r="B4" s="16">
-        <v>1.0500000000000006E-2</v>
-      </c>
-      <c r="C4">
-        <v>2.9000000000000002E-3</v>
-      </c>
-      <c r="D4" s="16">
-        <v>3.3000000000000002E-2</v>
-      </c>
-      <c r="E4">
-        <v>0.02</v>
+      <c r="B4" s="20">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="C4" s="19">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="D4" s="20">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="E4" s="19">
+        <v>2.3E-2</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I4" s="9" t="b">
+        <f>'GDPGR-alternate'!B2=Data!I3</f>
+        <v>1</v>
+      </c>
+      <c r="J4" s="9" t="b">
+        <f>'GDPGR-bau'!B2=Data!J3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>2022</v>
       </c>
       <c r="B5" s="16">
-        <v>1.3000000000000005E-2</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="C5">
-        <v>4.8000000000000004E-3</v>
+        <v>0.03</v>
       </c>
       <c r="D5" s="16">
-        <v>3.3000000000000002E-2</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="E5">
-        <v>0.02</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="9"/>
@@ -888,21 +933,21 @@
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>2023</v>
       </c>
       <c r="B6" s="16">
-        <v>1.5500000000000003E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="C6">
-        <v>6.7000000000000002E-3</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="D6" s="16">
-        <v>3.3000000000000002E-2</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="E6">
-        <v>0.02</v>
+        <v>2.4E-2</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="9"/>
@@ -910,21 +955,21 @@
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>2024</v>
       </c>
       <c r="B7" s="16">
-        <v>1.8000000000000002E-2</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="C7">
-        <v>8.6E-3</v>
+        <v>2.3E-2</v>
       </c>
       <c r="D7" s="16">
-        <v>3.3000000000000002E-2</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="E7">
-        <v>0.02</v>
+        <v>2.4E-2</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="9"/>
@@ -932,21 +977,21 @@
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>2025</v>
       </c>
       <c r="B8" s="16">
-        <v>2.0500000000000001E-2</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="C8">
-        <v>1.0500000000000001E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="D8" s="16">
-        <v>3.3000000000000002E-2</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="E8">
-        <v>0.02</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="F8" s="13"/>
       <c r="G8" s="12"/>
@@ -954,21 +999,21 @@
       <c r="I8" s="12"/>
       <c r="J8" s="12"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>2026</v>
       </c>
       <c r="B9" s="16">
-        <v>2.3E-2</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="C9">
-        <v>1.24E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="D9" s="16">
-        <v>3.3000000000000002E-2</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="E9">
-        <v>0.02</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="F9" s="13"/>
       <c r="G9" s="9"/>
@@ -976,21 +1021,21 @@
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>2027</v>
       </c>
       <c r="B10" s="16">
-        <v>2.5499999999999998E-2</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="C10">
-        <v>1.43E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="D10" s="16">
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="E10">
-        <v>0.02</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
@@ -998,21 +1043,21 @@
       <c r="I10" s="13"/>
       <c r="J10" s="13"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>2028</v>
       </c>
       <c r="B11" s="16">
-        <v>2.7999999999999997E-2</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="C11">
-        <v>1.6199999999999999E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="D11" s="16">
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="E11">
-        <v>0.02</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
@@ -1020,7 +1065,7 @@
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10">
       <c r="A12">
         <v>2029</v>
       </c>
@@ -1028,16 +1073,16 @@
         <v>3.0499999999999996E-2</v>
       </c>
       <c r="C12">
-        <v>1.8099999999999998E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="D12" s="16">
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="E12">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13">
         <v>2030</v>
       </c>
@@ -1054,7 +1099,7 @@
         <v>1.9999999999999997E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10">
       <c r="A14">
         <v>2031</v>
       </c>
@@ -1071,7 +1116,7 @@
         <v>1.9299999999999998E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10">
       <c r="A15">
         <v>2032</v>
       </c>
@@ -1088,7 +1133,7 @@
         <v>1.8599999999999998E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10">
       <c r="A16">
         <v>2033</v>
       </c>
@@ -1105,7 +1150,7 @@
         <v>1.7899999999999999E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>2034</v>
       </c>
@@ -1122,7 +1167,7 @@
         <v>1.7199999999999997E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>2035</v>
       </c>
@@ -1139,7 +1184,7 @@
         <v>1.6499999999999997E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>2036</v>
       </c>
@@ -1156,7 +1201,7 @@
         <v>1.5799999999999998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>2037</v>
       </c>
@@ -1173,7 +1218,7 @@
         <v>1.5099999999999999E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>2038</v>
       </c>
@@ -1190,7 +1235,7 @@
         <v>1.44E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>2039</v>
       </c>
@@ -1207,7 +1252,7 @@
         <v>1.37E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5">
       <c r="A23">
         <v>2040</v>
       </c>
@@ -1224,7 +1269,7 @@
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>2041</v>
       </c>
@@ -1241,7 +1286,7 @@
         <v>1.2699999999999999E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5">
       <c r="A25">
         <v>2042</v>
       </c>
@@ -1258,7 +1303,7 @@
         <v>1.24E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:5">
       <c r="A26">
         <v>2043</v>
       </c>
@@ -1275,7 +1320,7 @@
         <v>1.21E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:5">
       <c r="A27">
         <v>2044</v>
       </c>
@@ -1292,7 +1337,7 @@
         <v>1.18E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:5">
       <c r="A28">
         <v>2045</v>
       </c>
@@ -1309,7 +1354,7 @@
         <v>1.15E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:5">
       <c r="A29">
         <v>2046</v>
       </c>
@@ -1326,7 +1371,7 @@
         <v>1.1200000000000002E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:5">
       <c r="A30">
         <v>2047</v>
       </c>
@@ -1343,7 +1388,7 @@
         <v>1.09E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:5">
       <c r="A31">
         <v>2048</v>
       </c>
@@ -1360,7 +1405,7 @@
         <v>1.0600000000000002E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:5">
       <c r="A32">
         <v>2049</v>
       </c>
@@ -1377,7 +1422,7 @@
         <v>1.03E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:5">
       <c r="A33">
         <v>2050</v>
       </c>
@@ -1394,22 +1439,22 @@
         <v>1.0000000000000002E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:5">
       <c r="B34" s="17">
         <f>AVERAGE(B3:B33)</f>
-        <v>2.5032258064516134E-2</v>
+        <v>2.9080322580645166E-2</v>
       </c>
       <c r="C34" s="17">
         <f>AVERAGE(C3:C33)</f>
-        <v>1.2596774193548385E-2</v>
+        <v>1.6483870967741936E-2</v>
       </c>
       <c r="D34" s="17">
         <f>AVERAGE(D3:D33)</f>
-        <v>2.9467741935483877E-2</v>
+        <v>2.9532258064516134E-2</v>
       </c>
       <c r="E34" s="17">
         <f>AVERAGE(E3:E33)</f>
-        <v>1.5967741935483868E-2</v>
+        <v>1.6709677419354838E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1431,15 +1476,15 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="30.58203125" customWidth="1"/>
+    <col min="1" max="1" width="30.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2">
       <c r="A1" s="7" t="s">
         <v>14</v>
       </c>
@@ -1447,13 +1492,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="15">
-        <f>Data!C34</f>
-        <v>1.2596774193548385E-2</v>
+        <f>Data!$C$3</f>
+        <v>-8.9999999999999993E-3</v>
       </c>
     </row>
   </sheetData>
@@ -1469,16 +1514,16 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="30.58203125" customWidth="1"/>
+    <col min="1" max="1" width="30.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2">
       <c r="A1" s="7" t="s">
         <v>14</v>
       </c>
@@ -1486,13 +1531,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="15">
-        <f>Data!E34</f>
-        <v>1.5967741935483868E-2</v>
+        <f>Data!$E$3</f>
+        <v>0.02</v>
       </c>
     </row>
   </sheetData>

</xml_diff>